<commit_message>
Finished by adding the department filter
</commit_message>
<xml_diff>
--- a/prototype/templates/programme_dept_template.xlsx
+++ b/prototype/templates/programme_dept_template.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -447,32 +447,344 @@
           <t>Tech Fest</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Department of Computer Science</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Hackathon</t>
+          <t>Culture Fest</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Department of Cultural Studies</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Culture Fest</t>
+          <t>Commerce Fest</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Department of Commerce</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Commerce Fest</t>
-        </is>
-      </c>
+          <t>Hackathon</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Department of Computer Science</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Movie Fest</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Department of Computer Science, Department of Commerce, Department of Business Studies, Department of Cultural Studies"</formula1>
+      <formula1>"Department of Computer Science, Department of Commerce, Department of Business Studies, Department of Cultural Studies, Department of Media Communications"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added functionality to upload new users and programmes with departmentin excel template!
</commit_message>
<xml_diff>
--- a/prototype/templates/programme_dept_template.xlsx
+++ b/prototype/templates/programme_dept_template.xlsx
@@ -417,374 +417,40 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="24.28515625" customWidth="1" min="1" max="1"/>
-    <col width="37.140625" customWidth="1" min="2" max="2"/>
+    <col width="62.140625" customWidth="1" min="2" max="2"/>
+    <col width="37.140625" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Programme Name</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Department</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Tech Fest</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Department of Computer Science</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Culture Fest</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Department of Cultural Studies</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Commerce Fest</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Department of Business Studies</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Movie Fest</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Department of Media Communications</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Hackathon</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr"/>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr"/>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr"/>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr"/>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr"/>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr"/>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr"/>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr"/>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr"/>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr"/>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr"/>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr"/>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr"/>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr"/>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr"/>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr"/>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr"/>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr"/>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr"/>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr"/>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr"/>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr"/>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr"/>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr"/>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr"/>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr"/>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr"/>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr"/>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr"/>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr"/>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr"/>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr"/>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr"/>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr"/>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr"/>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr"/>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr"/>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr"/>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr"/>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr"/>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr"/>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr"/>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr"/>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr"/>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr"/>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr"/>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="B2:B100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Department of Computer Science, Department of Commerce, Department of Business Studies, Department of Cultural Studies, Department of Media Communications, Department of Arts"</formula1>
+    <dataValidation sqref="C2:C100" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Department of Computer Science, Department of Commerce, Department of Business Studies, Department of Cultural Studies, Department of Media Communications, Department of Arts, Department of Mathematics"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed excel data validation bug
</commit_message>
<xml_diff>
--- a/prototype/templates/programme_dept_template.xlsx
+++ b/prototype/templates/programme_dept_template.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="user_department" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="departments" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -419,7 +420,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -455,4 +456,94 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="36.7109375" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Department of Commerce</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Department of Business Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Department of Cultural Studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Department of Media Communications</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Department of Arts</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Department of Mathematics</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Department of Physical Education</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Department of Computer Science</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C100" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>'departments'!$A$2:$A$9</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>